<commit_message>
fixing some spreadsheets for imports
</commit_message>
<xml_diff>
--- a/tsp/Customers.xlsx
+++ b/tsp/Customers.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dde/sync/36109/Uber/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bambielli/simulation/tsp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A655DF3A-3B81-6141-9F39-23DE691819CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="1080" windowWidth="21020" windowHeight="16160" xr2:uid="{731C7BF9-FF07-6C45-9BD8-7FDBD277EC27}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -48,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -128,7 +133,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1660071</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
@@ -137,7 +142,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D021089B-1927-4543-943C-AB493C3635FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D021089B-1927-4543-943C-AB493C3635FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -478,11 +483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7BE902-386F-AA47-AB64-739AA78F2394}">
-  <dimension ref="A2:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,54 +497,54 @@
     <col min="3" max="5" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>33.780774999999998</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-84.386301000000003</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>33.780774999999998</v>
+        <v>33.776919999999997</v>
       </c>
       <c r="C3" s="3">
-        <v>-84.386301000000003</v>
+        <v>-84.389780000000002</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>33.776919999999997</v>
+        <v>33.773153999999998</v>
       </c>
       <c r="C4" s="3">
-        <v>-84.389780000000002</v>
+        <v>-84.397015999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>33.773153999999998</v>
-      </c>
-      <c r="C5" s="3">
-        <v>-84.397015999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>